<commit_message>
fix some bug and add breadcum
</commit_message>
<xml_diff>
--- a/tmp/user.xlsx
+++ b/tmp/user.xlsx
@@ -1,91 +1,164 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyunlu/code/go/projects/src/staff-mall-center/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19780FF-DA65-7E43-85C3-52B3EC458495}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>账号名称</t>
-  </si>
-  <si>
-    <t>user01</t>
-  </si>
-  <si>
-    <t>user02</t>
-  </si>
-  <si>
-    <t>user03</t>
-  </si>
-  <si>
-    <t>user04</t>
-  </si>
-  <si>
-    <t>用户名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户02</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户04</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>yangjunyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨俊彦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liyanwu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李炎伍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tangzhengwei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐政伟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yangwei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨维</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhengshen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑莘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nisha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>倪沙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liubin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘斌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pengjianguo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彭建国</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hanhuihua</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>韩慧华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuqiong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>付琼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhoutianfu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周天富</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiangzhongxin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江中信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linweiqiang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林伟强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fangcaixia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方彩霞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yangyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨宇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pengshuliang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彭姝靓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,10 +181,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -172,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -224,7 +295,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -418,83 +489,209 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="26.1" customHeight="1">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
         <v>123456</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
total product list operate
</commit_message>
<xml_diff>
--- a/tmp/user.xlsx
+++ b/tmp/user.xlsx
@@ -5,60 +5,134 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyunlu/code/go/projects/src/staff-mall-center/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyunlu/Postman/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19780FF-DA65-7E43-85C3-52B3EC458495}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8807F735-719C-364C-9AF7-61747C9A87F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28240" windowHeight="16080" xr2:uid="{AEC9261C-3F42-254D-94E7-61B30E9F517D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>账号名称</t>
-  </si>
-  <si>
-    <t>user01</t>
-  </si>
-  <si>
-    <t>user02</t>
-  </si>
-  <si>
-    <t>user03</t>
-  </si>
-  <si>
-    <t>user04</t>
-  </si>
-  <si>
-    <t>用户名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户02</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户04</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+  <si>
+    <t>商品简称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品全称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品类别简称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品类别全称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品库存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>苹果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fruit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麒麟瓜，500g一份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>milk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛奶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饮料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伊利优酸乳， 500ml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//img.yweidao.com/2017/07/18/goods_pc_image/1500354812152klo0txyvw3.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供应商(英文)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supplier01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供应商（全称）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxxx供应商</t>
+  </si>
+  <si>
+    <t>xxxx供应商</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supplier02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apple03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -67,25 +141,35 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF313131"/>
+      <name val="STHeiti"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,16 +189,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,76 +521,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F897EBA-FECE-7B49-BA69-061907E91ADC}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>123456</v>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>123456</v>
+    <row r="9" spans="1:10">
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://c-ssl.duitang.com/uploads/item/201208/26/20120826164510_y2nBQ.thumb.1400_0.jpeg" xr:uid="{7ACEC7E4-3440-9D49-87C9-211B96EC4468}"/>
+    <hyperlink ref="H3" r:id="rId2" display="http://img.yweidao.com/2017/07/18/goods_pc_image/1500354812152klo0txyvw3.jpg" xr:uid="{63A6B4CC-003C-E24D-BB72-449F16A4275C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>